<commit_message>
add payload for user password update and sample format
</commit_message>
<xml_diff>
--- a/sample-format/usersPost.xlsx
+++ b/sample-format/usersPost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B091F4-1DE2-4C34-A4E6-7AF50AC6DD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616BD520-616E-4A95-B92C-87D530C34856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1643,7 +1643,7 @@
   <dimension ref="A1:L142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A32"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>